<commit_message>
Made a html file of the thermal conductivity table
</commit_message>
<xml_diff>
--- a/project-1/Thermal_Conductivity_Calculator.xlsx
+++ b/project-1/Thermal_Conductivity_Calculator.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MY PC\Desktop\Resume\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kasulaverse\Kasulaverse-beta\Portfolio\Portfolio-Attempt-24-Thermal\project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -874,18 +874,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1023,117 +1017,98 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="24">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1160,21 +1135,7 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -1246,6 +1207,35 @@
           <bgColor theme="5"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <font>
@@ -1499,10 +1489,10 @@
   <autoFilter ref="B49:D50"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Heat Flux Unit" dataDxfId="9"/>
-    <tableColumn id="5" name="Q using (W/mK)" dataDxfId="1">
+    <tableColumn id="5" name="Q using (W/mK)" dataDxfId="8">
       <calculatedColumnFormula>C42*E17/E29</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" name="Q using (BTU/hr ft °F)" dataDxfId="0">
+    <tableColumn id="2" name="Q using (BTU/hr ft °F)" dataDxfId="7">
       <calculatedColumnFormula>(F42/E29)*E17</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1511,16 +1501,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B9:F127" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B9:F127" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="B9:F127"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Sl.no" dataDxfId="6">
+    <tableColumn id="1" name="Sl.no" dataDxfId="4">
       <calculatedColumnFormula>ROW(A1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Element Symbol" dataDxfId="5"/>
-    <tableColumn id="2" name="Element Name" dataDxfId="4"/>
-    <tableColumn id="4" name="Thermal Conductivity (W/mK)" dataDxfId="3"/>
-    <tableColumn id="5" name="Thermal Conductivity (BTU/hr ft °F)" dataDxfId="2"/>
+    <tableColumn id="3" name="Element Symbol" dataDxfId="3"/>
+    <tableColumn id="2" name="Element Name" dataDxfId="2"/>
+    <tableColumn id="4" name="Thermal Conductivity (W/mK)" dataDxfId="1" dataCellStyle="Normal"/>
+    <tableColumn id="5" name="Thermal Conductivity (BTU/hr ft °F)" dataDxfId="0" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1792,7 +1782,7 @@
   <dimension ref="B2:O50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E50" sqref="E50"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1807,110 +1797,110 @@
   <sheetData>
     <row r="2" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="16"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="16"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="18"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="19"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="16"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="19"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="18"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="19"/>
     </row>
     <row r="7" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="21"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="22"/>
     </row>
     <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="23" t="s">
         <v>250</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27"/>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="31"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
@@ -1977,27 +1967,27 @@
     </row>
     <row r="21" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="25"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="25"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="27"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="28"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="30"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="31"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
@@ -2149,95 +2139,95 @@
     </row>
     <row r="36" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="23" t="s">
         <v>263</v>
       </c>
-      <c r="C37" s="23"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="D37" s="24"/>
+      <c r="E37" s="24"/>
+      <c r="F37" s="25"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="25"/>
-      <c r="C38" s="26"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="27"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="28"/>
     </row>
     <row r="39" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="30"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="31"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="6" t="s">
+      <c r="B41" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D41" s="11"/>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11" t="s">
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="12">
+        <v>6</v>
+      </c>
+      <c r="C42" s="13">
         <f>INDEX('Thermal Conductivity Values'!E10:E127,MATCH(Calculator!B42,'Thermal Conductivity Values'!D10:D127,0))</f>
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12">
+        <v>0.18</v>
+      </c>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13">
         <f>INDEX('Thermal Conductivity Values'!F10:F127,MATCH(Calculator!B42,'Thermal Conductivity Values'!D10:D127,0))</f>
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
+        <v>0.104</v>
+      </c>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
     </row>
     <row r="44" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="45" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="C45" s="32"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
-      <c r="I45" s="33"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="10"/>
+      <c r="F45" s="10"/>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="11"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="4" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="6" t="s">
         <v>264</v>
       </c>
-      <c r="C50" s="8">
+      <c r="C50" s="7">
         <f>C42*E17/E29</f>
-        <v>35</v>
-      </c>
-      <c r="D50" s="10">
+        <v>128.57142857142858</v>
+      </c>
+      <c r="D50" s="8">
         <f>(F42/E29)*E17</f>
-        <v>20.000000000000004</v>
+        <v>74.285714285714292</v>
       </c>
     </row>
   </sheetData>
@@ -2278,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:P127"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J125" sqref="J125"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2292,101 +2282,101 @@
   <sheetData>
     <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="16"/>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="17"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="18"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="19"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C5" s="16"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="18"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="19"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="C6" s="16"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="18"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="19"/>
     </row>
     <row r="7" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="21"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="22"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2401,10 +2391,10 @@
       <c r="D10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="7">
         <v>0.18</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="7">
         <v>0.104</v>
       </c>
     </row>
@@ -2419,10 +2409,10 @@
       <c r="D11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="7">
         <v>0.151</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="7">
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
@@ -2437,10 +2427,10 @@
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="7">
         <v>84.8</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="7">
         <v>49</v>
       </c>
     </row>
@@ -2455,10 +2445,10 @@
       <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="7">
         <v>190</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="7">
         <v>110</v>
       </c>
     </row>
@@ -2473,10 +2463,10 @@
       <c r="D14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="7">
         <v>27</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="7">
         <v>15.6</v>
       </c>
     </row>
@@ -2491,10 +2481,10 @@
       <c r="D15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="7">
         <v>140</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="7">
         <v>81</v>
       </c>
     </row>
@@ -2509,10 +2499,10 @@
       <c r="D16" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="7">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="7">
         <v>1.4E-2</v>
       </c>
     </row>
@@ -2527,10 +2517,10 @@
       <c r="D17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="7">
         <v>2.4E-2</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="7">
         <v>1.4E-2</v>
       </c>
     </row>
@@ -2545,10 +2535,10 @@
       <c r="D18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="7">
         <v>2.7E-2</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="7">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -2563,10 +2553,10 @@
       <c r="D19" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="7">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="7">
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
@@ -2581,10 +2571,10 @@
       <c r="D20" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="7">
         <v>142</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="7">
         <v>82.2</v>
       </c>
     </row>
@@ -2599,10 +2589,10 @@
       <c r="D21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="7">
         <v>160</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="7">
         <v>92.8</v>
       </c>
     </row>
@@ -2617,10 +2607,10 @@
       <c r="D22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="7">
         <v>237</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="7">
         <v>137.19999999999999</v>
       </c>
     </row>
@@ -2635,10 +2625,10 @@
       <c r="D23" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="7">
         <v>149</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="7">
         <v>86.3</v>
       </c>
     </row>
@@ -2653,10 +2643,10 @@
       <c r="D24" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="7">
         <v>0.23599999999999999</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="7">
         <v>0.13600000000000001</v>
       </c>
     </row>
@@ -2671,10 +2661,10 @@
       <c r="D25" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="7">
         <v>0.20499999999999999</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="7">
         <v>0.11799999999999999</v>
       </c>
     </row>
@@ -2689,10 +2679,10 @@
       <c r="D26" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="7">
         <v>8.8999999999999999E-3</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="7">
         <v>5.1000000000000004E-3</v>
       </c>
     </row>
@@ -2707,10 +2697,10 @@
       <c r="D27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="7">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="7">
         <v>9.7999999999999997E-3</v>
       </c>
     </row>
@@ -2725,10 +2715,10 @@
       <c r="D28" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="7">
         <v>102</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="7">
         <v>59.1</v>
       </c>
     </row>
@@ -2743,10 +2733,10 @@
       <c r="D29" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="7">
         <v>200</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="7">
         <v>116</v>
       </c>
     </row>
@@ -2761,10 +2751,10 @@
       <c r="D30" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="7">
         <v>16</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="7">
         <v>9.3000000000000007</v>
       </c>
     </row>
@@ -2779,10 +2769,10 @@
       <c r="D31" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="7">
         <v>22</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="7">
         <v>12.7</v>
       </c>
     </row>
@@ -2797,10 +2787,10 @@
       <c r="D32" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="7">
         <v>31</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="7">
         <v>18</v>
       </c>
     </row>
@@ -2815,10 +2805,10 @@
       <c r="D33" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="7">
         <v>93</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="7">
         <v>53.8</v>
       </c>
     </row>
@@ -2833,10 +2823,10 @@
       <c r="D34" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="7">
         <v>7.8</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="7">
         <v>4.5</v>
       </c>
     </row>
@@ -2851,10 +2841,10 @@
       <c r="D35" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="7">
         <v>80</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="7">
         <v>46.4</v>
       </c>
     </row>
@@ -2869,10 +2859,10 @@
       <c r="D36" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="7">
         <v>100</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="7">
         <v>58</v>
       </c>
     </row>
@@ -2887,10 +2877,10 @@
       <c r="D37" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="7">
         <v>91.7</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="7">
         <v>53</v>
       </c>
     </row>
@@ -2905,10 +2895,10 @@
       <c r="D38" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="7">
         <v>401</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="7">
         <v>232</v>
       </c>
     </row>
@@ -2923,10 +2913,10 @@
       <c r="D39" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="7">
         <v>116</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="7">
         <v>67.2</v>
       </c>
     </row>
@@ -2941,10 +2931,10 @@
       <c r="D40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="7">
         <v>29.7</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="7">
         <v>17.2</v>
       </c>
     </row>
@@ -2959,10 +2949,10 @@
       <c r="D41" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="7">
         <v>60</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="7">
         <v>34.799999999999997</v>
       </c>
     </row>
@@ -2977,10 +2967,10 @@
       <c r="D42" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="7">
         <v>50</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="7">
         <v>29</v>
       </c>
     </row>
@@ -2995,10 +2985,10 @@
       <c r="D43" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="7">
         <v>0.52300000000000002</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="7">
         <v>0.30199999999999999</v>
       </c>
     </row>
@@ -3013,10 +3003,10 @@
       <c r="D44" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="7">
         <v>0.122</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="7">
         <v>7.0499999999999993E-2</v>
       </c>
     </row>
@@ -3031,10 +3021,10 @@
       <c r="D45" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="7">
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="7">
         <v>5.4000000000000003E-3</v>
       </c>
     </row>
@@ -3049,10 +3039,10 @@
       <c r="D46" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="7">
         <v>58.2</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="7">
         <v>33.700000000000003</v>
       </c>
     </row>
@@ -3067,10 +3057,10 @@
       <c r="D47" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="7">
         <v>35.4</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="7">
         <v>20.5</v>
       </c>
     </row>
@@ -3085,10 +3075,10 @@
       <c r="D48" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="7">
         <v>17.2</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48" s="7">
         <v>9.9600000000000009</v>
       </c>
     </row>
@@ -3103,10 +3093,10 @@
       <c r="D49" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49" s="7">
         <v>22.7</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="7">
         <v>13.1</v>
       </c>
     </row>
@@ -3121,10 +3111,10 @@
       <c r="D50" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="7">
         <v>53</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50" s="7">
         <v>30.6</v>
       </c>
     </row>
@@ -3139,10 +3129,10 @@
       <c r="D51" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51" s="7">
         <v>138</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F51" s="7">
         <v>79.8</v>
       </c>
     </row>
@@ -3157,11 +3147,11 @@
       <c r="D52" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E52" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F52" s="9">
-        <v>5000</v>
+      <c r="E52" s="7">
+        <v>50.6</v>
+      </c>
+      <c r="F52" s="7">
+        <v>29.4</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
@@ -3175,10 +3165,10 @@
       <c r="D53" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53" s="7">
         <v>117</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F53" s="7">
         <v>67.599999999999994</v>
       </c>
     </row>
@@ -3193,10 +3183,10 @@
       <c r="D54" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="7">
         <v>150</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F54" s="7">
         <v>86.8</v>
       </c>
     </row>
@@ -3211,10 +3201,10 @@
       <c r="D55" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55" s="7">
         <v>72.8</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F55" s="7">
         <v>42</v>
       </c>
     </row>
@@ -3229,10 +3219,10 @@
       <c r="D56" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="7">
         <v>429</v>
       </c>
-      <c r="F56" s="2">
+      <c r="F56" s="7">
         <v>248</v>
       </c>
     </row>
@@ -3247,10 +3237,10 @@
       <c r="D57" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57" s="7">
         <v>96.6</v>
       </c>
-      <c r="F57" s="2">
+      <c r="F57" s="7">
         <v>55.8</v>
       </c>
     </row>
@@ -3265,10 +3255,10 @@
       <c r="D58" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="7">
         <v>82.5</v>
       </c>
-      <c r="F58" s="2">
+      <c r="F58" s="7">
         <v>47.6</v>
       </c>
     </row>
@@ -3283,10 +3273,10 @@
       <c r="D59" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59" s="7">
         <v>66.8</v>
       </c>
-      <c r="F59" s="2">
+      <c r="F59" s="7">
         <v>38.6</v>
       </c>
     </row>
@@ -3301,10 +3291,10 @@
       <c r="D60" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60" s="7">
         <v>24.4</v>
       </c>
-      <c r="F60" s="2">
+      <c r="F60" s="7">
         <v>14.1</v>
       </c>
     </row>
@@ -3319,10 +3309,10 @@
       <c r="D61" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61" s="7">
         <v>3</v>
       </c>
-      <c r="F61" s="2">
+      <c r="F61" s="7">
         <v>1.73</v>
       </c>
     </row>
@@ -3337,10 +3327,10 @@
       <c r="D62" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62" s="7">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F62" s="2">
+      <c r="F62" s="7">
         <v>2.5999999999999999E-2</v>
       </c>
     </row>
@@ -3355,10 +3345,10 @@
       <c r="D63" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63" s="7">
         <v>5.6499999999999996E-3</v>
       </c>
-      <c r="F63" s="2">
+      <c r="F63" s="7">
         <v>3.2599999999999999E-3</v>
       </c>
     </row>
@@ -3373,10 +3363,10 @@
       <c r="D64" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64" s="7">
         <v>35.9</v>
       </c>
-      <c r="F64" s="2">
+      <c r="F64" s="7">
         <v>20.8</v>
       </c>
     </row>
@@ -3391,10 +3381,10 @@
       <c r="D65" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65" s="7">
         <v>18.399999999999999</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F65" s="7">
         <v>10.6</v>
       </c>
     </row>
@@ -3409,10 +3399,10 @@
       <c r="D66" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66" s="7">
         <v>13.4</v>
       </c>
-      <c r="F66" s="2">
+      <c r="F66" s="7">
         <v>7.74</v>
       </c>
     </row>
@@ -3427,10 +3417,10 @@
       <c r="D67" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67" s="7">
         <v>11.3</v>
       </c>
-      <c r="F67" s="2">
+      <c r="F67" s="7">
         <v>6.52</v>
       </c>
     </row>
@@ -3445,10 +3435,10 @@
       <c r="D68" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68" s="7">
         <v>13.7</v>
       </c>
-      <c r="F68" s="2">
+      <c r="F68" s="7">
         <v>7.91</v>
       </c>
     </row>
@@ -3463,10 +3453,10 @@
       <c r="D69" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69" s="7">
         <v>16.5</v>
       </c>
-      <c r="F69" s="2">
+      <c r="F69" s="7">
         <v>9.52</v>
       </c>
     </row>
@@ -3481,11 +3471,11 @@
       <c r="D70" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E70" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F70" s="9">
-        <v>5000</v>
+      <c r="E70" s="7">
+        <v>13.9</v>
+      </c>
+      <c r="F70" s="7">
+        <v>8.1</v>
       </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.3">
@@ -3499,10 +3489,10 @@
       <c r="D71" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71" s="7">
         <v>13.3</v>
       </c>
-      <c r="F71" s="2">
+      <c r="F71" s="7">
         <v>7.68</v>
       </c>
     </row>
@@ -3517,10 +3507,10 @@
       <c r="D72" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72" s="7">
         <v>13</v>
       </c>
-      <c r="F72" s="2">
+      <c r="F72" s="7">
         <v>7.5</v>
       </c>
     </row>
@@ -3535,10 +3525,10 @@
       <c r="D73" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73" s="7">
         <v>10.6</v>
       </c>
-      <c r="F73" s="2">
+      <c r="F73" s="7">
         <v>6.11</v>
       </c>
     </row>
@@ -3553,10 +3543,10 @@
       <c r="D74" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74" s="7">
         <v>11.1</v>
       </c>
-      <c r="F74" s="2">
+      <c r="F74" s="7">
         <v>6.41</v>
       </c>
     </row>
@@ -3571,10 +3561,10 @@
       <c r="D75" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75" s="7">
         <v>10.7</v>
       </c>
-      <c r="F75" s="2">
+      <c r="F75" s="7">
         <v>6.18</v>
       </c>
     </row>
@@ -3589,10 +3579,10 @@
       <c r="D76" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76" s="7">
         <v>16.2</v>
       </c>
-      <c r="F76" s="2">
+      <c r="F76" s="7">
         <v>9.35</v>
       </c>
     </row>
@@ -3607,10 +3597,10 @@
       <c r="D77" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77" s="7">
         <v>14.5</v>
       </c>
-      <c r="F77" s="2">
+      <c r="F77" s="7">
         <v>8.3699999999999992</v>
       </c>
     </row>
@@ -3625,10 +3615,10 @@
       <c r="D78" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E78" s="2">
+      <c r="E78" s="7">
         <v>16</v>
       </c>
-      <c r="F78" s="2">
+      <c r="F78" s="7">
         <v>9.24</v>
       </c>
     </row>
@@ -3643,10 +3633,10 @@
       <c r="D79" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79" s="7">
         <v>38</v>
       </c>
-      <c r="F79" s="2">
+      <c r="F79" s="7">
         <v>21.9</v>
       </c>
     </row>
@@ -3661,10 +3651,10 @@
       <c r="D80" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E80" s="7">
         <v>16.399999999999999</v>
       </c>
-      <c r="F80" s="2">
+      <c r="F80" s="7">
         <v>9.4700000000000006</v>
       </c>
     </row>
@@ -3679,10 +3669,10 @@
       <c r="D81" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E81" s="7">
         <v>23</v>
       </c>
-      <c r="F81" s="2">
+      <c r="F81" s="7">
         <v>13.3</v>
       </c>
     </row>
@@ -3697,10 +3687,10 @@
       <c r="D82" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82" s="7">
         <v>57.5</v>
       </c>
-      <c r="F82" s="2">
+      <c r="F82" s="7">
         <v>33.200000000000003</v>
       </c>
     </row>
@@ -3715,10 +3705,10 @@
       <c r="D83" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83" s="7">
         <v>173</v>
       </c>
-      <c r="F83" s="2">
+      <c r="F83" s="7">
         <v>100</v>
       </c>
     </row>
@@ -3733,10 +3723,10 @@
       <c r="D84" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84" s="7">
         <v>47.9</v>
       </c>
-      <c r="F84" s="2">
+      <c r="F84" s="7">
         <v>27.6</v>
       </c>
     </row>
@@ -3751,10 +3741,10 @@
       <c r="D85" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85" s="7">
         <v>87.6</v>
       </c>
-      <c r="F85" s="2">
+      <c r="F85" s="7">
         <v>50.5</v>
       </c>
     </row>
@@ -3769,10 +3759,10 @@
       <c r="D86" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="E86" s="2">
+      <c r="E86" s="7">
         <v>147</v>
       </c>
-      <c r="F86" s="2">
+      <c r="F86" s="7">
         <v>85</v>
       </c>
     </row>
@@ -3787,10 +3777,10 @@
       <c r="D87" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87" s="7">
         <v>71.599999999999994</v>
       </c>
-      <c r="F87" s="2">
+      <c r="F87" s="7">
         <v>41.3</v>
       </c>
     </row>
@@ -3805,10 +3795,10 @@
       <c r="D88" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88" s="7">
         <v>318</v>
       </c>
-      <c r="F88" s="2">
+      <c r="F88" s="7">
         <v>183</v>
       </c>
     </row>
@@ -3823,10 +3813,10 @@
       <c r="D89" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89" s="7">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F89" s="2">
+      <c r="F89" s="7">
         <v>4.79</v>
       </c>
     </row>
@@ -3841,10 +3831,10 @@
       <c r="D90" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90" s="7">
         <v>46.1</v>
       </c>
-      <c r="F90" s="2">
+      <c r="F90" s="7">
         <v>26.6</v>
       </c>
     </row>
@@ -3859,10 +3849,10 @@
       <c r="D91" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91" s="7">
         <v>35.299999999999997</v>
       </c>
-      <c r="F91" s="2">
+      <c r="F91" s="7">
         <v>20.399999999999999</v>
       </c>
     </row>
@@ -3877,10 +3867,10 @@
       <c r="D92" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92" s="7">
         <v>7.87</v>
       </c>
-      <c r="F92" s="2">
+      <c r="F92" s="7">
         <v>4.54</v>
       </c>
     </row>
@@ -3895,10 +3885,10 @@
       <c r="D93" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E93" s="2">
+      <c r="E93" s="7">
         <v>20</v>
       </c>
-      <c r="F93" s="2">
+      <c r="F93" s="7">
         <v>11.5</v>
       </c>
     </row>
@@ -3913,11 +3903,11 @@
       <c r="D94" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="E94" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F94" s="9">
-        <v>5000</v>
+      <c r="E94" s="7">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="F94" s="7">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.3">
@@ -3931,10 +3921,10 @@
       <c r="D95" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E95" s="2">
+      <c r="E95" s="7">
         <v>3.6099999999999999E-3</v>
       </c>
-      <c r="F95" s="2">
+      <c r="F95" s="7">
         <v>2.0799999999999998E-3</v>
       </c>
     </row>
@@ -3949,11 +3939,11 @@
       <c r="D96" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E96" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F96" s="9">
-        <v>5000</v>
+      <c r="E96" s="7">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F96" s="7">
+        <v>8.0999999999999996E-3</v>
       </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.3">
@@ -3967,10 +3957,10 @@
       <c r="D97" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E97" s="7">
         <v>19.899999999999999</v>
       </c>
-      <c r="F97" s="2">
+      <c r="F97" s="7">
         <v>11.5</v>
       </c>
     </row>
@@ -3985,10 +3975,10 @@
       <c r="D98" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E98" s="2">
+      <c r="E98" s="7">
         <v>12</v>
       </c>
-      <c r="F98" s="2">
+      <c r="F98" s="7">
         <v>6.92</v>
       </c>
     </row>
@@ -4003,10 +3993,10 @@
       <c r="D99" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E99" s="2">
+      <c r="E99" s="7">
         <v>54</v>
       </c>
-      <c r="F99" s="2">
+      <c r="F99" s="7">
         <v>31.2</v>
       </c>
     </row>
@@ -4021,10 +4011,10 @@
       <c r="D100" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E100" s="2">
+      <c r="E100" s="7">
         <v>47</v>
       </c>
-      <c r="F100" s="2">
+      <c r="F100" s="7">
         <v>27.1</v>
       </c>
     </row>
@@ -4039,10 +4029,10 @@
       <c r="D101" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E101" s="2">
+      <c r="E101" s="7">
         <v>27</v>
       </c>
-      <c r="F101" s="2">
+      <c r="F101" s="7">
         <v>15.6</v>
       </c>
     </row>
@@ -4057,11 +4047,11 @@
       <c r="D102" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E102" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F102" s="9">
-        <v>5000</v>
+      <c r="E102" s="7">
+        <v>6</v>
+      </c>
+      <c r="F102" s="7">
+        <v>3.49</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.3">
@@ -4075,10 +4065,10 @@
       <c r="D103" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E103" s="2">
+      <c r="E103" s="7">
         <v>6.74</v>
       </c>
-      <c r="F103" s="2">
+      <c r="F103" s="7">
         <v>3.89</v>
       </c>
     </row>
@@ -4093,10 +4083,10 @@
       <c r="D104" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="E104" s="2">
+      <c r="E104" s="7">
         <v>10</v>
       </c>
-      <c r="F104" s="2">
+      <c r="F104" s="7">
         <v>5.78</v>
       </c>
     </row>
@@ -4111,10 +4101,10 @@
       <c r="D105" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E105" s="2">
+      <c r="E105" s="7">
         <v>10.3</v>
       </c>
-      <c r="F105" s="2">
+      <c r="F105" s="7">
         <v>5.94</v>
       </c>
     </row>
@@ -4129,11 +4119,11 @@
       <c r="D106" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E106" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F106" s="9">
-        <v>5000</v>
+      <c r="E106" s="7">
+        <v>10</v>
+      </c>
+      <c r="F106" s="7">
+        <v>5.78</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.3">
@@ -4147,10 +4137,10 @@
       <c r="D107" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E107" s="2">
+      <c r="E107" s="7">
         <v>9.67</v>
       </c>
-      <c r="F107" s="2">
+      <c r="F107" s="7">
         <v>5.58</v>
       </c>
     </row>
@@ -4165,11 +4155,11 @@
       <c r="D108" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E108" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F108" s="9">
-        <v>5000</v>
+      <c r="E108" s="7">
+        <v>10</v>
+      </c>
+      <c r="F108" s="7">
+        <v>5.78</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.3">
@@ -4183,11 +4173,11 @@
       <c r="D109" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E109" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F109" s="9">
-        <v>5000</v>
+      <c r="E109" s="7">
+        <v>10</v>
+      </c>
+      <c r="F109" s="7">
+        <v>5.78</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.3">
@@ -4201,11 +4191,11 @@
       <c r="D110" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E110" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F110" s="9">
-        <v>5000</v>
+      <c r="E110" s="7">
+        <v>10</v>
+      </c>
+      <c r="F110" s="7">
+        <v>5.78</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.3">
@@ -4219,11 +4209,11 @@
       <c r="D111" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E111" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F111" s="9">
-        <v>5000</v>
+      <c r="E111" s="7">
+        <v>10</v>
+      </c>
+      <c r="F111" s="7">
+        <v>5.78</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.3">
@@ -4237,11 +4227,11 @@
       <c r="D112" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E112" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F112" s="9">
-        <v>5000</v>
+      <c r="E112" s="7">
+        <v>10</v>
+      </c>
+      <c r="F112" s="7">
+        <v>5.78</v>
       </c>
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.3">
@@ -4255,10 +4245,10 @@
       <c r="D113" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E113" s="2">
+      <c r="E113" s="7">
         <v>150</v>
       </c>
-      <c r="F113" s="2">
+      <c r="F113" s="7">
         <v>86.8</v>
       </c>
     </row>
@@ -4273,11 +4263,11 @@
       <c r="D114" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="E114" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F114" s="9">
-        <v>5000</v>
+      <c r="E114" s="7">
+        <v>268</v>
+      </c>
+      <c r="F114" s="7">
+        <v>156</v>
       </c>
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.3">
@@ -4291,11 +4281,11 @@
       <c r="D115" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E115" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F115" s="9">
-        <v>5000</v>
+      <c r="E115" s="7">
+        <v>271</v>
+      </c>
+      <c r="F115" s="7">
+        <v>158</v>
       </c>
     </row>
     <row r="116" spans="2:6" x14ac:dyDescent="0.3">
@@ -4309,11 +4299,11 @@
       <c r="D116" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="E116" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F116" s="9">
-        <v>5000</v>
+      <c r="E116" s="7">
+        <v>270</v>
+      </c>
+      <c r="F116" s="7">
+        <v>157</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.3">
@@ -4327,11 +4317,11 @@
       <c r="D117" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E117" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F117" s="9">
-        <v>5000</v>
+      <c r="E117" s="7">
+        <v>277</v>
+      </c>
+      <c r="F117" s="7">
+        <v>162</v>
       </c>
     </row>
     <row r="118" spans="2:6" x14ac:dyDescent="0.3">
@@ -4345,11 +4335,11 @@
       <c r="D118" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E118" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F118" s="9">
-        <v>5000</v>
+      <c r="E118" s="7">
+        <v>278</v>
+      </c>
+      <c r="F118" s="7">
+        <v>162</v>
       </c>
     </row>
     <row r="119" spans="2:6" x14ac:dyDescent="0.3">
@@ -4363,11 +4353,11 @@
       <c r="D119" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E119" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F119" s="9">
-        <v>5000</v>
+      <c r="E119" s="7">
+        <v>281</v>
+      </c>
+      <c r="F119" s="7">
+        <v>163</v>
       </c>
     </row>
     <row r="120" spans="2:6" x14ac:dyDescent="0.3">
@@ -4381,11 +4371,11 @@
       <c r="D120" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="E120" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F120" s="9">
-        <v>5000</v>
+      <c r="E120" s="7">
+        <v>282</v>
+      </c>
+      <c r="F120" s="7">
+        <v>165</v>
       </c>
     </row>
     <row r="121" spans="2:6" x14ac:dyDescent="0.3">
@@ -4399,11 +4389,11 @@
       <c r="D121" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E121" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F121" s="9">
-        <v>5000</v>
+      <c r="E121" s="7">
+        <v>285</v>
+      </c>
+      <c r="F121" s="7">
+        <v>167</v>
       </c>
     </row>
     <row r="122" spans="2:6" x14ac:dyDescent="0.3">
@@ -4417,11 +4407,11 @@
       <c r="D122" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E122" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F122" s="9">
-        <v>5000</v>
+      <c r="E122" s="7">
+        <v>284</v>
+      </c>
+      <c r="F122" s="7">
+        <v>175</v>
       </c>
     </row>
     <row r="123" spans="2:6" x14ac:dyDescent="0.3">
@@ -4435,11 +4425,11 @@
       <c r="D123" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E123" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F123" s="9">
-        <v>5000</v>
+      <c r="E123" s="7">
+        <v>289</v>
+      </c>
+      <c r="F123" s="7">
+        <v>170</v>
       </c>
     </row>
     <row r="124" spans="2:6" x14ac:dyDescent="0.3">
@@ -4453,11 +4443,11 @@
       <c r="D124" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E124" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F124" s="9">
-        <v>5000</v>
+      <c r="E124" s="7">
+        <v>288</v>
+      </c>
+      <c r="F124" s="7">
+        <v>173</v>
       </c>
     </row>
     <row r="125" spans="2:6" x14ac:dyDescent="0.3">
@@ -4471,11 +4461,11 @@
       <c r="D125" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="E125" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F125" s="9">
-        <v>5000</v>
+      <c r="E125" s="7">
+        <v>293</v>
+      </c>
+      <c r="F125" s="7">
+        <v>174</v>
       </c>
     </row>
     <row r="126" spans="2:6" x14ac:dyDescent="0.3">
@@ -4489,11 +4479,11 @@
       <c r="D126" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="E126" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F126" s="9">
-        <v>5000</v>
+      <c r="E126" s="7">
+        <v>294</v>
+      </c>
+      <c r="F126" s="7">
+        <v>176</v>
       </c>
     </row>
     <row r="127" spans="2:6" x14ac:dyDescent="0.3">
@@ -4507,27 +4497,17 @@
       <c r="D127" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="E127" s="9">
-        <v>5000</v>
-      </c>
-      <c r="F127" s="9">
-        <v>5000</v>
+      <c r="E127" s="7">
+        <v>294</v>
+      </c>
+      <c r="F127" s="7">
+        <v>176</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C3:P7"/>
   </mergeCells>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="5000"/>
-        <cfvo type="num" val="5000"/>
-        <color rgb="FFFF7128"/>
-        <color rgb="FFFFEF9C"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>